<commit_message>
project notification template changes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44018F0-D6E7-459A-BF17-2350C98C10F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4881A4E4-FC3C-421F-AD04-C10F87678CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Events!$A$1:$M$70</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$E$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$F$15</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="208">
   <si>
     <t>No</t>
   </si>
@@ -640,9 +640,6 @@
     <t>{"work_state": "COMPLETED"}</t>
   </si>
   <si>
-    <t>[{"phase_name":"Revised Project Notification Development","work_type_id": 6, "ea_act_id": 3, "event_name": "Meeting with Proponent", "is_active": false }]</t>
-  </si>
-  <si>
     <t>Set "Notification Review | Project Notification Submission Received (Day Zero)" ANTICIPATED to thisActual + 0</t>
   </si>
   <si>
@@ -655,16 +652,22 @@
     <t>{"work_type":  2}</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised Project Notification Development","work_type_id": 1, "ea_act_id": 3, "event_name": "Start of Intake Phase (e.g. Initial Contact, Draft Sharing, or PN Submission)", "start_at": 28 }</t>
-  </si>
-  <si>
     <t>#3eb1d7</t>
   </si>
   <si>
     <t>addPhase "Revised Project Notification Development" (this is a renamed copy of "Notification Intake"), addPhase "Revised Notification Review" and set phaseLegislated to FALSE (this is a renamed copy of "Notification Review"), addPhase "Revised Notification Decision" and set phaseLegislated to FALSE (this is a renamed copy of "Notification Decision")</t>
   </si>
   <si>
-    <t>[{"phase_name":"Notification Intake","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Project Notification Development", "legislated": false },{"phase_name":"Revised Project Notification Development","work_type_id": 6, "ea_act_id": 3, "event_name": "Meeting with Proponent", "is_active": false }, {"phase_name":"Notification Decision","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Notification Decision", "legislated": false }]</t>
+    <t>OutcomeDescription</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Notification Intake","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Project Notification Development", "legislated": false },{"phase_name":"Notification Review","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Notification Review", "legislated": false }, {"phase_name":"Notification Decision","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Notification Decision", "legislated": false }]</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Revised Project Notification Development","work_type_id": 1, "ea_act_id": 3, "event_name": "Meeting with Proponent", "is_active": false }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised Project Notification Development","work_type_id": 1, "ea_act_id": 3, "event_name": "Start of Intake Phase (e.g. Initial Contact, Draft Sharing, or PN Submission)", "start_at": 1 }</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>12</v>
@@ -1272,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>12</v>
@@ -1301,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>12</v>
@@ -2005,14 +2008,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -2071,7 +2073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1">
+    <row r="2" spans="1:13">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2110,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1">
+    <row r="3" spans="1:13">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2188,7 +2190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:13">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2227,7 +2229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1">
+    <row r="7" spans="1:13">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1">
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2347,7 +2349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2386,7 +2388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3931,7 +3933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1">
+    <row r="48" spans="1:13">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3970,7 +3972,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1">
+    <row r="49" spans="1:13">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -4009,7 +4011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1">
+    <row r="50" spans="1:13">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -4051,7 +4053,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1">
+    <row r="51" spans="1:13">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -4090,7 +4092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1">
+    <row r="52" spans="1:13">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -4129,7 +4131,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1">
+    <row r="53" spans="1:13">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4171,7 +4173,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1">
+    <row r="54" spans="1:13">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4213,7 +4215,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1">
+    <row r="55" spans="1:13">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4252,7 +4254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1">
+    <row r="56" spans="1:13">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4294,7 +4296,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1">
+    <row r="57" spans="1:13">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4336,7 +4338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1">
+    <row r="58" spans="1:13">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4375,7 +4377,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1">
+    <row r="59" spans="1:13">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4417,7 +4419,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" hidden="1">
+    <row r="60" spans="1:13">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4459,7 +4461,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1">
+    <row r="61" spans="1:13">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1">
+    <row r="62" spans="1:13">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4540,7 +4542,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1">
+    <row r="63" spans="1:13">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4582,7 +4584,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1">
+    <row r="64" spans="1:13">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4621,7 +4623,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1">
+    <row r="65" spans="1:13">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4663,7 +4665,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1">
+    <row r="66" spans="1:13">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4705,7 +4707,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1">
+    <row r="67" spans="1:13">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -4744,7 +4746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1">
+    <row r="68" spans="1:13">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -4783,7 +4785,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1">
+    <row r="69" spans="1:13">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -4825,7 +4827,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1">
+    <row r="70" spans="1:13">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -4868,13 +4870,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M70" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Notification Review"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M70" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="H1:H70">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
@@ -4931,25 +4927,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="6.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.7265625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="70.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="3" max="5" width="70.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1">
+    <row r="1" spans="1:7" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4963,10 +4959,13 @@
         <v>102</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4980,11 +4979,11 @@
       <c r="D2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4998,11 +4997,11 @@
       <c r="D3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5016,11 +5015,12 @@
       <c r="D4" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="19"/>
+      <c r="F4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5034,11 +5034,11 @@
       <c r="D5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5052,11 +5052,12 @@
       <c r="D6" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="19"/>
+      <c r="F6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5070,12 +5071,12 @@
       <c r="D7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>6</v>
       </c>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5089,11 +5090,11 @@
       <c r="D8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5107,11 +5108,12 @@
       <c r="D9" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="19"/>
+      <c r="F9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -5125,11 +5127,12 @@
       <c r="D10" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="19"/>
+      <c r="F10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -5143,11 +5146,12 @@
       <c r="D11" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="19"/>
+      <c r="F11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -5161,11 +5165,12 @@
       <c r="D12" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="19"/>
+      <c r="F12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -5179,11 +5184,11 @@
       <c r="D13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -5197,11 +5202,12 @@
       <c r="D14" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="19"/>
+      <c r="F14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5215,12 +5221,13 @@
       <c r="D15" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="19"/>
+      <c r="F15" s="2">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E15" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:F15" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -5241,11 +5248,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -5394,10 +5401,10 @@
         <v>126</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G6" s="1">
         <v>5</v>
@@ -5970,10 +5977,10 @@
         <v>135</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="G30" s="2">
         <v>29</v>
@@ -5997,7 +6004,7 @@
         <v>136</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="G31" s="2">
         <v>30</v>
@@ -6018,10 +6025,10 @@
         <v>126</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G32" s="2">
         <v>31</v>
@@ -6069,7 +6076,7 @@
         <v>138</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G34" s="2">
         <v>33</v>
@@ -7724,6 +7731,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2C1F259FB5F1743B0AABDE6E19F3587" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="887a673b2990ad08cbc7da39ce2412c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9da97c54-3012-49fd-8896-0db67528b2a3" xmlns:ns3="a10d9883-6879-4486-9776-c67b50dca88e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e318ef65ff943bae84f18b0edea6bb11" ns2:_="" ns3:_="">
     <xsd:import namespace="9da97c54-3012-49fd-8896-0db67528b2a3"/>
@@ -7952,27 +7979,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16DD9FF0-F1CC-4F04-BAE8-8534D757F315}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01AF64ED-2D5B-4E11-8E1C-2E238971D741}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548618B9-8BD2-484D-B813-9A3C00C2E6A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7989,23 +8015,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01AF64ED-2D5B-4E11-8E1C-2E238971D741}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16DD9FF0-F1CC-4F04-BAE8-8534D757F315}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Project notification template fix (#2146)
* should be able to filter work as active/inactive/all

* create_work not working

* project notification template changes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44018F0-D6E7-459A-BF17-2350C98C10F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFA3E71-3F10-44A2-8780-FBD4B4652930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Events!$A$1:$M$70</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$E$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$F$15</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="208">
   <si>
     <t>No</t>
   </si>
@@ -640,31 +640,34 @@
     <t>{"work_state": "COMPLETED"}</t>
   </si>
   <si>
-    <t>[{"phase_name":"Revised Project Notification Development","work_type_id": 6, "ea_act_id": 3, "event_name": "Meeting with Proponent", "is_active": false }]</t>
-  </si>
-  <si>
     <t>Set "Notification Review | Project Notification Submission Received (Day Zero)" ANTICIPATED to thisActual + 0</t>
   </si>
   <si>
-    <t>Set "Revised Project Notification Development | Start of Intake Phase" to thisEventACTUAL +28 (this is a renamed copy of "Start of Intake Phase (e.g. Initial Contact, Draft Sharing, or PN Submission)")</t>
-  </si>
-  <si>
     <t>{"phase_name":"Notification Review","work_type_id": 1, "ea_act_id": 3, "event_name": "Project Notification Submission Received (Day Zero)", "start_at": 0 }</t>
   </si>
   <si>
     <t>{"work_type":  2}</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised Project Notification Development","work_type_id": 1, "ea_act_id": 3, "event_name": "Start of Intake Phase (e.g. Initial Contact, Draft Sharing, or PN Submission)", "start_at": 28 }</t>
-  </si>
-  <si>
     <t>#3eb1d7</t>
   </si>
   <si>
     <t>addPhase "Revised Project Notification Development" (this is a renamed copy of "Notification Intake"), addPhase "Revised Notification Review" and set phaseLegislated to FALSE (this is a renamed copy of "Notification Review"), addPhase "Revised Notification Decision" and set phaseLegislated to FALSE (this is a renamed copy of "Notification Decision")</t>
   </si>
   <si>
-    <t>[{"phase_name":"Notification Intake","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Project Notification Development", "legislated": false },{"phase_name":"Revised Project Notification Development","work_type_id": 6, "ea_act_id": 3, "event_name": "Meeting with Proponent", "is_active": false }, {"phase_name":"Notification Decision","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Notification Decision", "legislated": false }]</t>
+    <t>OutcomeDescription</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Notification Intake","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Project Notification Development", "legislated": false },{"phase_name":"Notification Review","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Notification Review", "legislated": false }, {"phase_name":"Notification Decision","work_type_id": 1, "ea_act_id": 3, "new_name": "Revised Notification Decision", "legislated": false }]</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Revised Project Notification Development","work_type_id": 1, "ea_act_id": 3, "event_name": "Meeting with Proponent", "is_active": false }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised Project Notification Development","work_type_id": 1, "ea_act_id": 3, "event_name": "Start of Intake Phase (e.g. Initial Contact, Draft Sharing, or PN Submission)", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>Set "Revised Project Notification Development | Start of Intake Phase" to thisEventACTUAL +1 (this is a renamed copy of "Start of Intake Phase (e.g. Initial Contact, Draft Sharing, or PN Submission)")</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>12</v>
@@ -1272,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>12</v>
@@ -1301,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>12</v>
@@ -2005,14 +2008,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -2071,7 +2073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1">
+    <row r="2" spans="1:13">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2110,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1">
+    <row r="3" spans="1:13">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2188,7 +2190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1">
+    <row r="5" spans="1:13">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2227,7 +2229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1">
+    <row r="6" spans="1:13">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1">
+    <row r="7" spans="1:13">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1">
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2347,7 +2349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1">
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2386,7 +2388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3931,7 +3933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1">
+    <row r="48" spans="1:13">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3970,7 +3972,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1">
+    <row r="49" spans="1:13">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -4009,7 +4011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1">
+    <row r="50" spans="1:13">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -4051,7 +4053,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1">
+    <row r="51" spans="1:13">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -4090,7 +4092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1">
+    <row r="52" spans="1:13">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -4129,7 +4131,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1">
+    <row r="53" spans="1:13">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4171,7 +4173,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1">
+    <row r="54" spans="1:13">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4213,7 +4215,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1">
+    <row r="55" spans="1:13">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4252,7 +4254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1">
+    <row r="56" spans="1:13">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4294,7 +4296,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1">
+    <row r="57" spans="1:13">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4336,7 +4338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1">
+    <row r="58" spans="1:13">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4375,7 +4377,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1">
+    <row r="59" spans="1:13">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4417,7 +4419,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" hidden="1">
+    <row r="60" spans="1:13">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4459,7 +4461,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1">
+    <row r="61" spans="1:13">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1">
+    <row r="62" spans="1:13">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4540,7 +4542,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1">
+    <row r="63" spans="1:13">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4582,7 +4584,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1">
+    <row r="64" spans="1:13">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4621,7 +4623,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1">
+    <row r="65" spans="1:13">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4663,7 +4665,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1">
+    <row r="66" spans="1:13">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4705,7 +4707,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1">
+    <row r="67" spans="1:13">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -4744,7 +4746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1">
+    <row r="68" spans="1:13">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -4783,7 +4785,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1">
+    <row r="69" spans="1:13">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -4825,7 +4827,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1">
+    <row r="70" spans="1:13">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -4868,13 +4870,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M70" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Notification Review"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M70" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="H1:H70">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
@@ -4931,25 +4927,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="6.7265625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.7265625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="70.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="3" max="5" width="70.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1">
+    <row r="1" spans="1:7" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4963,10 +4959,13 @@
         <v>102</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4980,11 +4979,11 @@
       <c r="D2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4998,11 +4997,11 @@
       <c r="D3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5016,11 +5015,12 @@
       <c r="D4" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="19"/>
+      <c r="F4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5034,11 +5034,11 @@
       <c r="D5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5052,11 +5052,12 @@
       <c r="D6" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="19"/>
+      <c r="F6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5070,12 +5071,12 @@
       <c r="D7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>6</v>
       </c>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5089,11 +5090,11 @@
       <c r="D8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5107,11 +5108,12 @@
       <c r="D9" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="19"/>
+      <c r="F9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -5125,11 +5127,12 @@
       <c r="D10" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="19"/>
+      <c r="F10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -5143,11 +5146,12 @@
       <c r="D11" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="19"/>
+      <c r="F11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -5161,11 +5165,12 @@
       <c r="D12" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="19"/>
+      <c r="F12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -5179,11 +5184,11 @@
       <c r="D13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -5197,11 +5202,12 @@
       <c r="D14" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="19"/>
+      <c r="F14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5215,12 +5221,13 @@
       <c r="D15" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="19"/>
+      <c r="F15" s="2">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E15" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:F15" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -5242,10 +5249,10 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -5394,10 +5401,10 @@
         <v>126</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="G6" s="1">
         <v>5</v>
@@ -5970,10 +5977,10 @@
         <v>135</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G30" s="2">
         <v>29</v>
@@ -5997,7 +6004,7 @@
         <v>136</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="G31" s="2">
         <v>30</v>
@@ -6018,10 +6025,10 @@
         <v>126</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G32" s="2">
         <v>31</v>
@@ -6069,7 +6076,7 @@
         <v>138</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G34" s="2">
         <v>33</v>

</xml_diff>

<commit_message>
project notification phase number change
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFA3E71-3F10-44A2-8780-FBD4B4652930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACB3F44-9792-4512-AA69-94DC8891C82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -1183,7 +1183,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1269,7 +1269,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>1</v>
@@ -1298,7 +1298,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>1</v>
@@ -2010,11 +2010,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48:XFD48"/>
+      <selection pane="bottomRight" activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -3921,7 +3921,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K47" s="2">
         <v>0</v>
@@ -4773,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K68" s="2">
         <v>0</v>
@@ -5248,7 +5248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -7731,6 +7731,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2C1F259FB5F1743B0AABDE6E19F3587" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="887a673b2990ad08cbc7da39ce2412c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9da97c54-3012-49fd-8896-0db67528b2a3" xmlns:ns3="a10d9883-6879-4486-9776-c67b50dca88e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e318ef65ff943bae84f18b0edea6bb11" ns2:_="" ns3:_="">
     <xsd:import namespace="9da97c54-3012-49fd-8896-0db67528b2a3"/>
@@ -7959,15 +7968,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7980,6 +7980,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01AF64ED-2D5B-4E11-8E1C-2E238971D741}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548618B9-8BD2-484D-B813-9A3C00C2E6A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7998,14 +8006,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01AF64ED-2D5B-4E11-8E1C-2E238971D741}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16DD9FF0-F1CC-4F04-BAE8-8534D757F315}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
project notification phase number change (#2166)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/project_notification/002_Project_Notification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\project_notification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFA3E71-3F10-44A2-8780-FBD4B4652930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACB3F44-9792-4512-AA69-94DC8891C82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -1183,7 +1183,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1269,7 +1269,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>1</v>
@@ -1298,7 +1298,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>1</v>
@@ -2010,11 +2010,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48:XFD48"/>
+      <selection pane="bottomRight" activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -3921,7 +3921,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K47" s="2">
         <v>0</v>
@@ -4773,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K68" s="2">
         <v>0</v>
@@ -5248,7 +5248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -7731,6 +7731,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2C1F259FB5F1743B0AABDE6E19F3587" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="887a673b2990ad08cbc7da39ce2412c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9da97c54-3012-49fd-8896-0db67528b2a3" xmlns:ns3="a10d9883-6879-4486-9776-c67b50dca88e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e318ef65ff943bae84f18b0edea6bb11" ns2:_="" ns3:_="">
     <xsd:import namespace="9da97c54-3012-49fd-8896-0db67528b2a3"/>
@@ -7959,15 +7968,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7980,6 +7980,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01AF64ED-2D5B-4E11-8E1C-2E238971D741}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{548618B9-8BD2-484D-B813-9A3C00C2E6A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7998,14 +8006,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01AF64ED-2D5B-4E11-8E1C-2E238971D741}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16DD9FF0-F1CC-4F04-BAE8-8534D757F315}">
   <ds:schemaRefs>

</xml_diff>